<commit_message>
add date and time in add new order
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,34 +468,258 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>آیفون سیتی</t>
+          <t>موبایل جوان هشتگرد</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14752</t>
+          <t>1785</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1402-09-24</t>
+          <t>1402-10-22</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>23:50</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>پیک موتوری</t>
+          <t>پست</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>فاکتور : حسین رشیدی</t>
-        </is>
-      </c>
+          <t>فاکتور</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>موبایل جوان هشتگرد</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1402-10-22</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>18:02</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>پست</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>تست</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>موبایل جوان هشتگرد</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>121212</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1402-10-22</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18:02</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>پست</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>موبوپلاس ارومیه</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1402-10-22</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>12:27</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>پست</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>فروشگاه طنین موزیک</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>54545</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1402-10-22</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>17:58</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>پست</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>فروشگاه کامپیوتر R+</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>4565</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1402-10-19</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>17:55</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>پست</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>های استور</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1402-10-01</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>17:34</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>پست</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>مصطفی ساری</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1402-10-22</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>17:18</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>پست</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>موبایل جوان هشتگرد</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>11111</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1402-10-22</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>17:15</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>پست</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>